<commit_message>
Nueva actualización V2.2, arreglos en el guardado de precios
</commit_message>
<xml_diff>
--- a/precios.xlsx
+++ b/precios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="publico" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="estudiante" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="publico" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="estudiante" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,15 +520,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -539,18 +542,21 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C2" t="n">
+        <v>70</v>
+      </c>
+      <c r="D2" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2" t="n">
+        <v>60</v>
+      </c>
+      <c r="F2" t="n">
         <v>50</v>
       </c>
-      <c r="D2" t="n">
-        <v>50</v>
-      </c>
-      <c r="E2" t="n">
-        <v>40</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>40</v>
       </c>
     </row>
@@ -564,15 +570,18 @@
         <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
         <v>80</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F3" t="n">
+        <v>70</v>
+      </c>
+      <c r="G3" t="n">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ahora calcula según el total de paginas y no el de cada archivo, fallos en calculo manual
</commit_message>
<xml_diff>
--- a/precios.xlsx
+++ b/precios.xlsx
@@ -466,10 +466,10 @@
         <v>80</v>
       </c>
       <c r="D2" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E2" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -481,14 +481,12 @@
       <c r="B3" t="n">
         <v>100</v>
       </c>
-      <c r="C3" t="n">
-        <v>100</v>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
         <v>80</v>
       </c>
       <c r="E3" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -520,19 +518,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="n">
         <v>20</v>
       </c>
       <c r="E1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>100</v>
       </c>
     </row>
     <row r="2">
@@ -551,14 +549,12 @@
         <v>60</v>
       </c>
       <c r="E2" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
         <v>50</v>
       </c>
-      <c r="G2" t="n">
-        <v>40</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -569,20 +565,14 @@
       <c r="B3" t="n">
         <v>100</v>
       </c>
-      <c r="C3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D3" t="n">
-        <v>80</v>
-      </c>
-      <c r="E3" t="n">
-        <v>80</v>
-      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G3" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>